<commit_message>
Implemented MySQL commands to be sent to AWS for database implementation. Also testing web server.
</commit_message>
<xml_diff>
--- a/Diagrams/Gantt Chart.xlsx
+++ b/Diagrams/Gantt Chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryannguyen/Documents/SJSU/CMPE 195E/senior-project-195e/Diagrams/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryann\Documents\SJSU\Senior Project\senior-project-195e\Diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79FF5E16-5D16-8240-BA67-45CBFD4695E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57405337-21E8-4478-A670-C9A0DFB1711C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17380" activeTab="1" xr2:uid="{84B47839-57C0-EE42-AA37-BC5EA0291CB5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{84B47839-57C0-EE42-AA37-BC5EA0291CB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Group" sheetId="1" r:id="rId1"/>
@@ -1047,36 +1047,36 @@
   </sheetPr>
   <dimension ref="A1:AP31"/>
   <sheetViews>
-    <sheetView zoomScale="114" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="2.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="2.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="63.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="59.375" style="2" customWidth="1"/>
+    <col min="2" max="3" width="3.125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="3.125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="3.125" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="3.125" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="20" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="3.125" style="1" bestFit="1" customWidth="1"/>
     <col min="21" max="22" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="25" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="25" width="3.125" style="1" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="29" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="29" width="3.125" style="1" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="33" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="33" width="3.125" style="1" bestFit="1" customWidth="1"/>
     <col min="34" max="35" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="38" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="38" width="3.125" style="1" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="40" max="42" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="43" max="16384" width="2.83203125" style="1"/>
+    <col min="40" max="42" width="3.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="43" max="16384" width="2.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:42" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>64</v>
       </c>
@@ -1128,7 +1128,7 @@
       <c r="AO1" s="38"/>
       <c r="AP1" s="39"/>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
         <v>38</v>
       </c>
@@ -1194,7 +1194,7 @@
       <c r="AO2" s="40"/>
       <c r="AP2" s="41"/>
     </row>
-    <row r="3" spans="1:42" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:42" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
         <v>37</v>
       </c>
@@ -1363,7 +1363,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
         <v>25</v>
       </c>
@@ -1409,7 +1409,7 @@
       <c r="AO4" s="36"/>
       <c r="AP4" s="37"/>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A5" s="30" t="s">
         <v>23</v>
       </c>
@@ -1455,7 +1455,7 @@
       <c r="AO5" s="3"/>
       <c r="AP5" s="5"/>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
         <v>24</v>
       </c>
@@ -1501,7 +1501,7 @@
       <c r="AO6" s="3"/>
       <c r="AP6" s="5"/>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A7" s="30" t="s">
         <v>0</v>
       </c>
@@ -1547,7 +1547,7 @@
       <c r="AO7" s="3"/>
       <c r="AP7" s="5"/>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A8" s="30" t="s">
         <v>1</v>
       </c>
@@ -1593,7 +1593,7 @@
       <c r="AO8" s="3"/>
       <c r="AP8" s="5"/>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A9" s="30" t="s">
         <v>2</v>
       </c>
@@ -1639,7 +1639,7 @@
       <c r="AO9" s="3"/>
       <c r="AP9" s="5"/>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
         <v>20</v>
       </c>
@@ -1685,7 +1685,7 @@
       <c r="AO10" s="3"/>
       <c r="AP10" s="5"/>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A11" s="30" t="s">
         <v>3</v>
       </c>
@@ -1731,7 +1731,7 @@
       <c r="AO11" s="3"/>
       <c r="AP11" s="5"/>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A12" s="30" t="s">
         <v>4</v>
       </c>
@@ -1777,7 +1777,7 @@
       <c r="AO12" s="3"/>
       <c r="AP12" s="5"/>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A13" s="30" t="s">
         <v>21</v>
       </c>
@@ -1823,7 +1823,7 @@
       <c r="AO13" s="3"/>
       <c r="AP13" s="5"/>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A14" s="30" t="s">
         <v>5</v>
       </c>
@@ -1869,7 +1869,7 @@
       <c r="AO14" s="3"/>
       <c r="AP14" s="5"/>
     </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A15" s="30" t="s">
         <v>6</v>
       </c>
@@ -1915,7 +1915,7 @@
       <c r="AO15" s="3"/>
       <c r="AP15" s="5"/>
     </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A16" s="30" t="s">
         <v>22</v>
       </c>
@@ -1961,7 +1961,7 @@
       <c r="AO16" s="3"/>
       <c r="AP16" s="5"/>
     </row>
-    <row r="17" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A17" s="32" t="s">
         <v>41</v>
       </c>
@@ -2007,7 +2007,7 @@
       <c r="AO17" s="33"/>
       <c r="AP17" s="34"/>
     </row>
-    <row r="18" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A18" s="30" t="s">
         <v>26</v>
       </c>
@@ -2053,7 +2053,7 @@
       <c r="AO18" s="3"/>
       <c r="AP18" s="5"/>
     </row>
-    <row r="19" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A19" s="30" t="s">
         <v>28</v>
       </c>
@@ -2099,7 +2099,7 @@
       <c r="AO19" s="3"/>
       <c r="AP19" s="5"/>
     </row>
-    <row r="20" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A20" s="30" t="s">
         <v>27</v>
       </c>
@@ -2145,7 +2145,7 @@
       <c r="AO20" s="3"/>
       <c r="AP20" s="5"/>
     </row>
-    <row r="21" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A21" s="30" t="s">
         <v>29</v>
       </c>
@@ -2191,7 +2191,7 @@
       <c r="AO21" s="3"/>
       <c r="AP21" s="5"/>
     </row>
-    <row r="22" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A22" s="32" t="s">
         <v>39</v>
       </c>
@@ -2237,7 +2237,7 @@
       <c r="AO22" s="33"/>
       <c r="AP22" s="34"/>
     </row>
-    <row r="23" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A23" s="30" t="s">
         <v>30</v>
       </c>
@@ -2283,7 +2283,7 @@
       <c r="AO23" s="3"/>
       <c r="AP23" s="5"/>
     </row>
-    <row r="24" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A24" s="30" t="s">
         <v>31</v>
       </c>
@@ -2329,7 +2329,7 @@
       <c r="AO24" s="3"/>
       <c r="AP24" s="5"/>
     </row>
-    <row r="25" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A25" s="30" t="s">
         <v>52</v>
       </c>
@@ -2375,7 +2375,7 @@
       <c r="AO25" s="3"/>
       <c r="AP25" s="5"/>
     </row>
-    <row r="26" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A26" s="30" t="s">
         <v>32</v>
       </c>
@@ -2421,7 +2421,7 @@
       <c r="AO26" s="3"/>
       <c r="AP26" s="5"/>
     </row>
-    <row r="27" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A27" s="30" t="s">
         <v>33</v>
       </c>
@@ -2467,7 +2467,7 @@
       <c r="AO27" s="3"/>
       <c r="AP27" s="5"/>
     </row>
-    <row r="28" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A28" s="30" t="s">
         <v>34</v>
       </c>
@@ -2513,7 +2513,7 @@
       <c r="AO28" s="3"/>
       <c r="AP28" s="5"/>
     </row>
-    <row r="29" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A29" s="30" t="s">
         <v>36</v>
       </c>
@@ -2559,7 +2559,7 @@
       <c r="AO29" s="3"/>
       <c r="AP29" s="5"/>
     </row>
-    <row r="30" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A30" s="30" t="s">
         <v>35</v>
       </c>
@@ -2605,7 +2605,7 @@
       <c r="AO30" s="3"/>
       <c r="AP30" s="5"/>
     </row>
-    <row r="31" spans="1:42" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:42" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="31" t="s">
         <v>40</v>
       </c>
@@ -2672,7 +2672,7 @@
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="60" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup scale="60" orientation="landscape" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2683,35 +2683,35 @@
   </sheetPr>
   <dimension ref="A1:AN25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
-      <selection activeCell="AD8" sqref="AD8"/>
+    <sheetView zoomScale="114" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="2.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="2.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="63.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="63.625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="3.125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="3.125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="3.125" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="3.125" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="20" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="23" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="23" width="3.125" style="1" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="27" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="3.125" style="1" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="31" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="31" width="3.125" style="1" bestFit="1" customWidth="1"/>
     <col min="32" max="33" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="36" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="36" width="3.125" style="1" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="40" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="41" max="16384" width="2.83203125" style="1"/>
+    <col min="38" max="40" width="3.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="41" max="16384" width="2.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:40" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>65</v>
       </c>
@@ -2738,7 +2738,7 @@
       <c r="T1" s="38"/>
       <c r="U1" s="39"/>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
         <v>38</v>
       </c>
@@ -2773,7 +2773,7 @@
       <c r="T2" s="40"/>
       <c r="U2" s="41"/>
     </row>
-    <row r="3" spans="1:40" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
         <v>37</v>
       </c>
@@ -2858,7 +2858,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4" s="44" t="s">
         <v>43</v>
       </c>
@@ -2902,7 +2902,7 @@
       <c r="AM4"/>
       <c r="AN4"/>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>42</v>
       </c>
@@ -2946,7 +2946,7 @@
       <c r="AM5"/>
       <c r="AN5"/>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>48</v>
       </c>
@@ -2990,7 +2990,7 @@
       <c r="AM6"/>
       <c r="AN6"/>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>49</v>
       </c>
@@ -3034,7 +3034,7 @@
       <c r="AM7"/>
       <c r="AN7"/>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>56</v>
       </c>
@@ -3078,7 +3078,7 @@
       <c r="AM8"/>
       <c r="AN8"/>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>45</v>
       </c>
@@ -3122,7 +3122,7 @@
       <c r="AM9"/>
       <c r="AN9"/>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
         <v>53</v>
       </c>
@@ -3166,7 +3166,7 @@
       <c r="AM10"/>
       <c r="AN10"/>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>44</v>
       </c>
@@ -3210,7 +3210,7 @@
       <c r="AM11"/>
       <c r="AN11"/>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
         <v>59</v>
       </c>
@@ -3254,7 +3254,7 @@
       <c r="AM12"/>
       <c r="AN12"/>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>50</v>
       </c>
@@ -3298,7 +3298,7 @@
       <c r="AM13"/>
       <c r="AN13"/>
     </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
         <v>55</v>
       </c>
@@ -3325,7 +3325,7 @@
       <c r="V14"/>
       <c r="W14"/>
     </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
         <v>57</v>
       </c>
@@ -3352,7 +3352,7 @@
       <c r="V15"/>
       <c r="W15"/>
     </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
         <v>58</v>
       </c>
@@ -3379,7 +3379,7 @@
       <c r="V16"/>
       <c r="W16"/>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>51</v>
       </c>
@@ -3406,7 +3406,7 @@
       <c r="V17"/>
       <c r="W17"/>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
         <v>46</v>
       </c>
@@ -3432,7 +3432,7 @@
       <c r="U18" s="16"/>
       <c r="V18"/>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>47</v>
       </c>
@@ -3457,7 +3457,7 @@
       <c r="T19" s="14"/>
       <c r="U19" s="20"/>
     </row>
-    <row r="20" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="21" t="s">
         <v>54</v>
       </c>
@@ -3482,28 +3482,28 @@
       <c r="T20" s="23"/>
       <c r="U20" s="24"/>
     </row>
-    <row r="21" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21"/>
     </row>
-    <row r="22" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="42" t="s">
         <v>60</v>
       </c>
       <c r="B22" s="43"/>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>61</v>
       </c>
       <c r="B23" s="11"/>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>62</v>
       </c>
       <c r="B24" s="8"/>
     </row>
-    <row r="25" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>63</v>
       </c>

</xml_diff>